<commit_message>
feat: update Talent language
更新天赋元素克制相关数值，多语言，战斗倍速UI
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentBuff_天赋数值表.xlsx
+++ b/nevergiveup/Excel/TalentBuff_天赋数值表.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661573F3-4310-4B01-B2B0-DED1014E6BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426D73AD-288C-472C-8027-60B8DD734B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="166">
   <si>
     <t>int</t>
   </si>
@@ -252,16 +252,10 @@
     <t>黯灭</t>
   </si>
   <si>
-    <t>敌方入场5秒内护甲减少{0}</t>
-  </si>
-  <si>
     <t>TalentTree_Name_19</t>
   </si>
   <si>
     <t>希瓦</t>
-  </si>
-  <si>
-    <t>敌方入场5秒内魔抗减少{0}</t>
   </si>
   <si>
     <t>TalentTree_Name_20</t>
@@ -531,6 +525,22 @@
   </si>
   <si>
     <t>木·Ⅱ</t>
+  </si>
+  <si>
+    <t>10|20|30</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌方入场10秒内减速{0}%</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌方入场10秒内护甲减少{0}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌方入场10秒内魔抗减少{0}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -895,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -995,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -1018,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -1064,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
@@ -1110,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -1133,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -1156,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
@@ -1179,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
@@ -1225,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="1">
         <v>2</v>
@@ -1248,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
@@ -1271,7 +1281,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F17" s="1">
         <v>2</v>
@@ -1294,13 +1304,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F18" s="1">
         <v>2</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>61</v>
+      <c r="G18" s="6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
@@ -1317,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
@@ -1340,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F20" s="1">
         <v>2</v>
@@ -1386,13 +1396,13 @@
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>73</v>
+      <c r="G22" s="6" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -1400,22 +1410,22 @@
         <v>1019</v>
       </c>
       <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>76</v>
+      <c r="G23" s="6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -1423,22 +1433,22 @@
         <v>1020</v>
       </c>
       <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -1446,10 +1456,10 @@
         <v>1021</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1461,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -1469,22 +1479,22 @@
         <v>1022</v>
       </c>
       <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
@@ -1492,22 +1502,22 @@
         <v>1023</v>
       </c>
       <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
@@ -1515,16 +1525,16 @@
         <v>1024</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
@@ -1538,16 +1548,16 @@
         <v>1025</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F29" s="1">
         <v>2</v>
@@ -1561,16 +1571,16 @@
         <v>1026</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F30" s="1">
         <v>2</v>
@@ -1584,10 +1594,10 @@
         <v>1027</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1607,16 +1617,16 @@
         <v>1028</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F32" s="1">
         <v>2</v>
@@ -1630,10 +1640,10 @@
         <v>1029</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -1653,16 +1663,16 @@
         <v>1030</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -1676,16 +1686,16 @@
         <v>1031</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F35" s="1">
         <v>2</v>
@@ -1699,16 +1709,16 @@
         <v>1032</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F36" s="1">
         <v>2</v>
@@ -1722,16 +1732,16 @@
         <v>1033</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F37" s="1">
         <v>2</v>
@@ -1745,10 +1755,10 @@
         <v>1034</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -1768,16 +1778,16 @@
         <v>1035</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F39" s="1">
         <v>2</v>
@@ -1791,16 +1801,16 @@
         <v>1036</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F40" s="1">
         <v>2</v>
@@ -1814,16 +1824,16 @@
         <v>1037</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F41" s="1">
         <v>2</v>
@@ -1837,22 +1847,22 @@
         <v>1038</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F42" s="1">
         <v>2</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>61</v>
+      <c r="G42" s="6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
@@ -1860,16 +1870,16 @@
         <v>1039</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F43" s="1">
         <v>2</v>
@@ -1883,16 +1893,16 @@
         <v>1040</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F44" s="1">
         <v>2</v>
@@ -1906,10 +1916,10 @@
         <v>1041</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -1929,22 +1939,22 @@
         <v>1042</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>73</v>
+      <c r="G46" s="6" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.15">
@@ -1952,22 +1962,22 @@
         <v>1043</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>76</v>
+      <c r="G47" s="6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
@@ -1975,22 +1985,22 @@
         <v>1044</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F48" s="1">
         <v>2</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.15">
@@ -1998,10 +2008,10 @@
         <v>1045</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -2013,7 +2023,7 @@
         <v>2</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.15">
@@ -2021,16 +2031,16 @@
         <v>1046</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F50" s="1">
         <v>2</v>
@@ -2044,22 +2054,22 @@
         <v>1047</v>
       </c>
       <c r="B51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2</v>
+      </c>
+      <c r="E51" s="4">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="1">
-        <v>2</v>
-      </c>
-      <c r="E51" s="4">
-        <v>2</v>
-      </c>
-      <c r="F51" s="1">
-        <v>2</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.15">
@@ -2067,22 +2077,22 @@
         <v>1048</v>
       </c>
       <c r="B52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="4">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D52" s="1">
-        <v>2</v>
-      </c>
-      <c r="E52" s="4">
-        <v>2</v>
-      </c>
-      <c r="F52" s="1">
-        <v>2</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.15">
@@ -2090,10 +2100,10 @@
         <v>1049</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D53" s="1">
         <v>2</v>
@@ -2105,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.15">
@@ -2113,16 +2123,16 @@
         <v>2001</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F54" s="1">
         <v>2</v>
@@ -2136,16 +2146,16 @@
         <v>2002</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F55" s="1">
         <v>2</v>
@@ -2159,16 +2169,16 @@
         <v>2003</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F56" s="1">
         <v>2</v>
@@ -2182,16 +2192,16 @@
         <v>2004</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F57" s="1">
         <v>2</v>
@@ -2205,10 +2215,10 @@
         <v>2005</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
@@ -2228,16 +2238,16 @@
         <v>2006</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F59" s="1">
         <v>2</v>

</xml_diff>